<commit_message>
feat: data can be stored in file.xlsx
</commit_message>
<xml_diff>
--- a/src/server/visitors.xlsx
+++ b/src/server/visitors.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -433,10 +433,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>07-09-2024</v>
+        <v>08-09-2024</v>
       </c>
       <c r="B2" t="str">
-        <v>123</v>
+        <v>hlinhbk</v>
       </c>
       <c r="C2" t="str">
         <v/>
@@ -451,15 +451,67 @@
         <v/>
       </c>
       <c r="G2" t="str">
-        <v>2024-10-07</v>
+        <v>2024-10-08</v>
       </c>
       <c r="H2" t="str">
-        <v>2024-10-07</v>
+        <v>2024-10-08</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>08-09-2024</v>
+      </c>
+      <c r="B3" t="str">
+        <v>hlinhbk</v>
+      </c>
+      <c r="C3" t="str">
+        <v/>
+      </c>
+      <c r="D3" t="str">
+        <v/>
+      </c>
+      <c r="E3" t="str">
+        <v/>
+      </c>
+      <c r="F3" t="str">
+        <v/>
+      </c>
+      <c r="G3" t="str">
+        <v>2024-10-08</v>
+      </c>
+      <c r="H3" t="str">
+        <v>2024-10-08</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>08-09-2024</v>
+      </c>
+      <c r="B4" t="str">
+        <v>hlinhbk</v>
+      </c>
+      <c r="C4" t="str">
+        <v/>
+      </c>
+      <c r="D4" t="str">
+        <v/>
+      </c>
+      <c r="E4" t="str">
+        <v/>
+      </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
+      <c r="G4" t="str">
+        <v>2024-10-08</v>
+      </c>
+      <c r="H4" t="str">
+        <v>2024-10-08</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>